<commit_message>
Awards Secret directors fix
</commit_message>
<xml_diff>
--- a/awards_secret.xlsx
+++ b/awards_secret.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,11 +479,6 @@
           <t>Director</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>ear</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -522,13 +517,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Daniel Kwan
-Daniel Scheinert</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2022</t>
+          <t>Daniel Kwan, Daniel Scheinert</t>
         </is>
       </c>
     </row>
@@ -572,11 +561,6 @@
           <t>Edward Berger</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -618,11 +602,6 @@
           <t>Darren Aronofsky</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -664,11 +643,6 @@
           <t>Joseph Kosinski</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -710,11 +684,6 @@
           <t>Ryan Coogler</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -756,11 +725,6 @@
           <t>James Cameron</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -802,11 +766,6 @@
           <t>Sarah Polley</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -845,13 +804,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Guillermo del Toro
-Mark Gustafson</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>2022</t>
+          <t>Guillermo del Toro, Mark Gustafson</t>
         </is>
       </c>
     </row>
@@ -895,11 +848,6 @@
           <t>Daniel Roher</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -941,11 +889,6 @@
           <t>Kartiki Gonsalves</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -984,13 +927,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Tom Berkeley
-Ross White</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>2022</t>
+          <t>Tom Berkeley, Ross White</t>
         </is>
       </c>
     </row>
@@ -1031,13 +968,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Peter Baynton
-Charlie Mackesy</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>2022</t>
+          <t>Peter Baynton, Charlie Mackesy</t>
         </is>
       </c>
     </row>
@@ -1081,11 +1012,6 @@
           <t>S. S. Rajamouli</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1127,11 +1053,6 @@
           <t>Sian Heder</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1173,11 +1094,6 @@
           <t>Denis Villeneuve</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1219,11 +1135,6 @@
           <t>Michael Showalter</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1265,11 +1176,6 @@
           <t>Cary Joji Fukunaga</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1311,11 +1217,6 @@
           <t>Alberto Mielgo</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1353,11 +1254,6 @@
         <v>0</v>
       </c>
       <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1399,11 +1295,6 @@
           <t>Ben Proudfoot</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1445,11 +1336,6 @@
           <t>Ahmir "Questlove" Thompson</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1491,11 +1377,6 @@
           <t>Ryusuke Hamaguchi</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1534,13 +1415,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Jared Bush
-Byron Howard</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>2021</t>
+          <t>Jared Bush, Byron Howard</t>
         </is>
       </c>
     </row>
@@ -1584,11 +1459,6 @@
           <t>Steven Spielberg</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1630,11 +1500,6 @@
           <t>Kenneth Branagh</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1676,11 +1541,6 @@
           <t>Jane Campion</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1722,11 +1582,6 @@
           <t>Reinaldo Marcus Green</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1766,704 +1621,6 @@
       <c r="I29" t="inlineStr">
         <is>
           <t>Craig Gillespie</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Nomadland</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Nomadland_(film)</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
-        <v>5</v>
-      </c>
-      <c r="H30" t="n">
-        <v>39.5</v>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Chloé Zhao</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>The Father</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/The_Father_(2020_film)</t>
-        </is>
-      </c>
-      <c r="G31" t="n">
-        <v>6</v>
-      </c>
-      <c r="H31" t="n">
-        <v>36.4</v>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>Florian Zeller</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Judas and the Black Messiah</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Judas_and_the_Black_Messiah</t>
-        </is>
-      </c>
-      <c r="G32" t="n">
-        <v>26</v>
-      </c>
-      <c r="H32" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>Shaka King</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Minari</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Minari_(film)</t>
-        </is>
-      </c>
-      <c r="G33" t="n">
-        <v>2</v>
-      </c>
-      <c r="H33" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Lee Isaac Chung</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Mank</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Mank</t>
-        </is>
-      </c>
-      <c r="G34" t="n">
-        <v>25</v>
-      </c>
-      <c r="H34" t="n">
-        <v>122</v>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>David Fincher</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Sound of Metal</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Sound_of_Metal</t>
-        </is>
-      </c>
-      <c r="G35" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="H35" t="n">
-        <v>516</v>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>Darius Marder</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Ma Rainey's Black Bottom</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Ma_Rainey%27s_Black_Bottom_(film)</t>
-        </is>
-      </c>
-      <c r="G36" t="n">
-        <v>20</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>George C. Wolfe</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Promising Young Woman</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Promising_Young_Woman</t>
-        </is>
-      </c>
-      <c r="G37" t="n">
-        <v>10</v>
-      </c>
-      <c r="H37" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>Emerald Fennell</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Tenet</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Tenet_(film)</t>
-        </is>
-      </c>
-      <c r="G38" t="n">
-        <v>205</v>
-      </c>
-      <c r="H38" t="n">
-        <v>365.3</v>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>Christopher Nolan</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Soul</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Soul_(2020_film)</t>
-        </is>
-      </c>
-      <c r="G39" t="n">
-        <v>150</v>
-      </c>
-      <c r="H39" t="n">
-        <v>121</v>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>Pete Docter</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Another Round</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Another_Round_(film)</t>
-        </is>
-      </c>
-      <c r="G40" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="H40" t="n">
-        <v>21.7</v>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>Thomas Vinterberg</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>My Octopus Teacher</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/My_Octopus_Teacher</t>
-        </is>
-      </c>
-      <c r="G41" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>Pippa Ehrlich
-James Reed</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Colette</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Colette_(2020_film)</t>
-        </is>
-      </c>
-      <c r="G42" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>Anthony Giacchino</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>If Anything Happens I Love You</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/If_Anything_Happens_I_Love_You</t>
-        </is>
-      </c>
-      <c r="G43" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>Will McCormack
-Michael Govier</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Two Distant Strangers</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>2020/21</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Two_Distant_Strangers</t>
-        </is>
-      </c>
-      <c r="G44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" t="n">
-        <v>50</v>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>Travon Free
-Martin Desmond Roe</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>2020</t>
         </is>
       </c>
     </row>

</xml_diff>